<commit_message>
realeseing the first full version of the GUI program working perfectly , still have problems when working on another windows , need to create employee names configration file
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F30A40C-0257-4BF5-8E4E-515296BCDDBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347D629E-5576-4BF1-B0FC-4C939DC5814B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="12930" windowHeight="5640" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="5640" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>رند 25-05</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,8 +443,8 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finally Fix the Selenium Crash Error when browser windows lost focus , the solution is to use --headless=new  in the config file for both chrome and edge
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347D629E-5576-4BF1-B0FC-4C939DC5814B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7B1962-B7BB-45EF-9384-C7F27B41E7B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="5640" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
   </bookViews>
@@ -39,19 +39,19 @@
     <t>is_random</t>
   </si>
   <si>
-    <t>05-11</t>
-  </si>
-  <si>
     <t>05-25</t>
   </si>
   <si>
-    <t>احمد 11-05</t>
-  </si>
-  <si>
-    <t>رند 25-05</t>
-  </si>
-  <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>01-01</t>
+  </si>
+  <si>
+    <t>جيانا</t>
+  </si>
+  <si>
+    <t>رند</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,29 +434,29 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="str">
+        <f>"C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A2&amp;" "&amp;C2</f>
+        <v>C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\samples\جيانا 01-01</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="str">
-        <f>"C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A2</f>
-        <v>C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\samples\احمد 11-05</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="str">
-        <f>"C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A3</f>
-        <v>C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\samples\رند 25-05</v>
+        <f>"C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A3&amp;" "&amp;C3</f>
+        <v>C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\samples\رند 05-25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
return --headless=new para to cfg file
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Documents\Projects\OPOST_AUTOMATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DEC147-4265-415B-9223-6AD45866D678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E5C9BE-51FC-4E33-94E6-61BF5AF54A29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
   </bookViews>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -419,7 +408,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,8 +437,8 @@
         <v>7</v>
       </c>
       <c r="B2" t="str">
-        <f>"C:\Users\moham\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A2&amp;" "&amp;C2</f>
-        <v>C:\Users\moham\Documents\Projects\OPOST_AUTOMATION\samples\جيانا 01-01</v>
+        <f>"C:\Users\AL-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A2&amp;" "&amp;C2</f>
+        <v>C:\Users\AL-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\جيانا 01-01</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -463,8 +452,8 @@
         <v>8</v>
       </c>
       <c r="B3" t="str">
-        <f>"C:\Users\moham\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A3&amp;" "&amp;C3</f>
-        <v>C:\Users\moham\Documents\Projects\OPOST_AUTOMATION\samples\رند 05-25</v>
+        <f>"C:\Users\al-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A3&amp;" "&amp;C3</f>
+        <v>C:\Users\al-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\رند 05-25</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Delete All Unnecessary excel files
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E5C9BE-51FC-4E33-94E6-61BF5AF54A29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4EB1A7-DFAE-4BC0-88EA-5912947EB557}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -39,19 +39,13 @@
     <t>is_random</t>
   </si>
   <si>
-    <t>05-25</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
-    <t>01-01</t>
-  </si>
-  <si>
     <t>جيانا</t>
   </si>
   <si>
-    <t>رند</t>
+    <t>02-03</t>
   </si>
 </sst>
 </file>
@@ -405,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE93E2F7-E7E8-4115-BDA6-BC182164122C}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,32 +428,17 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="str">
         <f>"C:\Users\AL-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A2&amp;" "&amp;C2</f>
-        <v>C:\Users\AL-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\جيانا 01-01</v>
+        <v>C:\Users\AL-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\جيانا 02-03</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="str">
-        <f>"C:\Users\al-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A3&amp;" "&amp;C3</f>
-        <v>C:\Users\al-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\رند 05-25</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Format Columns and Cells For Final Results report [column widths]
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4EB1A7-DFAE-4BC0-88EA-5912947EB557}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E6EBA8-DBF6-427E-9605-2A8A40629083}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
   </bookViews>
@@ -39,13 +39,13 @@
     <t>is_random</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>جيانا</t>
-  </si>
-  <si>
-    <t>02-03</t>
+    <t>ديما</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>02-02</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,17 +428,17 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="str">
         <f>"C:\Users\AL-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A2&amp;" "&amp;C2</f>
-        <v>C:\Users\AL-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\جيانا 02-03</v>
+        <v>C:\Users\AL-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\ديما 02-02</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solve browser update issue and remove redundant code
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Documents\Projects\OPOST_AUTOMATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E6EBA8-DBF6-427E-9605-2A8A40629083}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526AE8F8-EC60-440D-9276-1808DCB15CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -402,17 +402,17 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="91.28515625" customWidth="1"/>
-    <col min="3" max="4" width="22.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="91.33203125" customWidth="1"/>
+    <col min="3" max="4" width="22.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,13 +426,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="str">
-        <f>"C:\Users\AL-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\"&amp;A2&amp;" "&amp;C2</f>
-        <v>C:\Users\AL-thuraya\Documents\Projects\OPOST_AUTOMATION\samples\ديما 02-02</v>
+        <f>"samples\"&amp;A2&amp;" "&amp;C2</f>
+        <v>samples\ديما 02-02</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
fix the cod count bug by removing cod_count_per_user and deliver cod count directly in excel there was a problem in the BLCB-VJU-004773778 shipment
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Documents\Projects\OPOST_AUTOMATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526AE8F8-EC60-440D-9276-1808DCB15CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9245FE0F-2D5C-440F-BC4E-C6D982D0202F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>02-02</t>
+  </si>
+  <si>
+    <t>جيانا</t>
   </si>
 </sst>
 </file>
@@ -399,20 +402,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE93E2F7-E7E8-4115-BDA6-BC182164122C}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="91.33203125" customWidth="1"/>
-    <col min="3" max="4" width="22.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="91.28515625" customWidth="1"/>
+    <col min="3" max="4" width="22.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,7 +429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -438,6 +441,21 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"samples\"&amp;A3&amp;" "&amp;C3</f>
+        <v>samples\جيانا 02-02</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove unnecessary comments , remove unused codes , change the port to 9333 , Still having problems in bad connection and slow OPOST response
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AL-Thuraya\Documents\Projects\OPOST_AUTOMATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Documents\Projects\OPOST_AUTOMATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9245FE0F-2D5C-440F-BC4E-C6D982D0202F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6BB6D9-F23D-4F3E-A19F-612C7669FCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>ديما</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>02-02</t>
@@ -55,9 +52,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="178"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -85,9 +90,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,62 +410,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE93E2F7-E7E8-4115-BDA6-BC182164122C}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="91.28515625" customWidth="1"/>
-    <col min="3" max="4" width="22.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="91.33203125" customWidth="1"/>
+    <col min="3" max="4" width="22.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="2" t="str">
         <f>"samples\"&amp;A2&amp;" "&amp;C2</f>
         <v>samples\ديما 02-02</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="str">
+      <c r="B3" s="2" t="str">
         <f>"samples\"&amp;A3&amp;" "&amp;C3</f>
         <v>samples\جيانا 02-02</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
create a sample selector menu ,remove unncessary codes , The perfect fix of any chrome versions issue is to update chrome manually from browser settings
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Documents\Projects\OPOST_AUTOMATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6BB6D9-F23D-4F3E-A19F-612C7669FCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFF398E-DF46-410F-8897-D1900448C29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>is_random</t>
-  </si>
-  <si>
-    <t>ديما</t>
   </si>
   <si>
     <t>02-02</t>
@@ -410,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE93E2F7-E7E8-4115-BDA6-BC182164122C}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,42 +436,30 @@
     </row>
     <row r="2" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>"samples\"&amp;A2&amp;" "&amp;C2</f>
-        <v>samples\ديما 02-02</v>
+        <v>samples\جيانا 02-02</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f>"samples\"&amp;A3&amp;" "&amp;C3</f>
-        <v>samples\جيانا 02-02</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D5" s="4"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D6" s="4"/>
@@ -511,6 +496,9 @@
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix empty list (division by zero) in  createExcel function if no results were retrieved  (no pendings found)
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Documents\Projects\OPOST_AUTOMATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Al-Thuraya\Documents\Projects\OPOST_AUTOMATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFF398E-DF46-410F-8897-D1900448C29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB79E2E8-3E5D-4CD8-8323-8DCEE41CB48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{76656C06-CAC6-4619-8517-418B521C5DF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -39,10 +39,13 @@
     <t>is_random</t>
   </si>
   <si>
-    <t>02-02</t>
+    <t>جيانا</t>
   </si>
   <si>
-    <t>جيانا</t>
+    <t>حمزة</t>
+  </si>
+  <si>
+    <t>04-13</t>
   </si>
 </sst>
 </file>
@@ -53,7 +56,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -61,7 +64,7 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -87,12 +90,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,98 +411,432 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE93E2F7-E7E8-4115-BDA6-BC182164122C}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="91.33203125" customWidth="1"/>
-    <col min="3" max="4" width="22.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="91.375" customWidth="1"/>
+    <col min="3" max="3" width="22.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>"samples\"&amp;A2&amp;" "&amp;C2</f>
-        <v>samples\جيانا 02-02</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3">
+        <v>samples\جيانا 04-13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="5" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f t="shared" ref="B3:B44" si="0">"samples\"&amp;A3&amp;" "&amp;C3</f>
+        <v>samples\حمزة 04-13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C11" s="3"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="2"/>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2"/>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="2"/>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="2"/>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="2"/>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="2"/>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="2"/>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="2"/>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="2"/>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="2"/>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">samples\ </v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>